<commit_message>
v1.2.2 save excel data and add english vocabulary
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/chat_content_20200512.xlsx
+++ b/ai/assets/textbook/chat_content_20200512.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3480D3E0-6E73-4D34-872A-555F2D3784DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545991FD-E324-4EE0-951C-7AEAF3EDE1D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31050" yWindow="3600" windowWidth="25890" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29580" yWindow="780" windowWidth="25890" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="382">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -572,6 +572,680 @@
   </si>
   <si>
     <t>不</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>懂得趣玩躲喑@  花奇  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>玩躲喑@  花奇  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>玩躲喑@  板罗  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>666上分卡鱼就系躲晕号   管家鱼</t>
+  </si>
+  <si>
+    <t>atm sang</t>
+  </si>
+  <si>
+    <t>B A TCCTV</t>
+  </si>
+  <si>
+    <t>bye无空格yao{77}</t>
+  </si>
+  <si>
+    <t>dvd  稳扌dao{65}</t>
+  </si>
+  <si>
+    <t>DVD 小晓COV</t>
+  </si>
+  <si>
+    <t>dvd 机会dao 徽{65}</t>
+  </si>
+  <si>
+    <t>dvd 恋曲dao 徽{65}</t>
+  </si>
+  <si>
+    <t>DVD不干活 COV</t>
+  </si>
+  <si>
+    <t>DVD连着啊COV</t>
+  </si>
+  <si>
+    <t>DVD连着COV</t>
+  </si>
+  <si>
+    <t>tun 财神送金 nao</t>
+  </si>
+  <si>
+    <t>tun财神嫁到nao</t>
+  </si>
+  <si>
+    <t>tun救星威nao</t>
+  </si>
+  <si>
+    <t>two前面的off后面</t>
+  </si>
+  <si>
+    <t>v,如可哥，拼，都懂的</t>
+  </si>
+  <si>
+    <t>XBB视讯</t>
+  </si>
+  <si>
+    <t>ㄨ??767薯片</t>
+  </si>
+  <si>
+    <t>ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>ㄨ??356</t>
+  </si>
+  <si>
+    <t>ㄨ??168</t>
+  </si>
+  <si>
+    <t>ㄨ??552</t>
+  </si>
+  <si>
+    <t>人人都有机会看你抓不抓得住了徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>人人看好都有钻徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>刀了躲音@ 花奇  那播了</t>
+  </si>
+  <si>
+    <t>上分卡鱼就系躲晕号   管家鱼</t>
+  </si>
+  <si>
+    <t>上分回复徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>上分徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>上暗??????</t>
+  </si>
+  <si>
+    <t>上暗躺赢徽??????</t>
+  </si>
+  <si>
+    <t>大师待赢钱不难徴狺  ?444 ?ㄨ机会不要错过</t>
+  </si>
+  <si>
+    <t>大家去捕鱼乐园好打</t>
+  </si>
+  <si>
+    <t>不上分的，1玩躲喑@  花奇  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>不上头的抱团法则 徴狺  ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>不要上头莱可樂这抱团 徴狺  ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>今天收工咯目标到了别自己瞎玩了试试吧 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>今天收工咯目标完成其实赢钱真的不难 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>今天吴我收工咯目标完成啦其实真的不难赢 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>反正自己玩不好哪有那么多钱输不如试试 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>开心今天收工咯目标到了别自己瞎玩了试试吧 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>乧愔，鲨鱼走兽@直播扑鱼了。</t>
+  </si>
+  <si>
+    <t>乧愔，闗驻，鲨鱼走兽，直播扑鱼。</t>
+  </si>
+  <si>
+    <t>仔下DCD练起YOU</t>
+  </si>
+  <si>
+    <t>乧愔，鲨鱼走兽@直播扑鱼绞敩了。。</t>
+  </si>
+  <si>
+    <t>卡鱼上分就系躲晕号    管家鱼</t>
+  </si>
+  <si>
+    <t>卡点爆分躲晕@管家鱼，快乐扑鱼</t>
+  </si>
+  <si>
+    <t>可徽关注 AG大姐姐，偷偷告诉好方法永远不输钱啊</t>
+  </si>
+  <si>
+    <t>扑才再躲音 欢快濮鱼开课啦啦</t>
+  </si>
+  <si>
+    <t>扑 才再躲音 开课值波中</t>
+  </si>
+  <si>
+    <t>扑 才再躲音 濮鱼开始啦</t>
+  </si>
+  <si>
+    <t>伐内幕消息好方法徽关注 AG大哥</t>
+  </si>
+  <si>
+    <t>光驻 芒果仙女</t>
+  </si>
+  <si>
+    <t>光祝ぇ芒果仙女</t>
+  </si>
+  <si>
+    <t>全打 语纹 扌并 奔马哥</t>
+  </si>
+  <si>
+    <t>全英{8}西安牛神</t>
+  </si>
+  <si>
+    <t>全英威 奔马各  线下搭伙</t>
+  </si>
+  <si>
+    <t>关注-路线王子</t>
+  </si>
+  <si>
+    <t>关注我，隔壁东叔</t>
+  </si>
+  <si>
+    <t>再下DCD联起YOU</t>
+  </si>
+  <si>
+    <t>吃肉会会徽??967?抓图吃</t>
+  </si>
+  <si>
+    <t>吃肉的??353?{89}</t>
+  </si>
+  <si>
+    <t>吃肉家会??962? 吃肉</t>
+  </si>
+  <si>
+    <t>吃肉随我 ??981?</t>
+  </si>
+  <si>
+    <t>吃香香徽??962?</t>
+  </si>
+  <si>
+    <t>妇内幕消息好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>早上好早班车差两个徴狺  ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>有大把大神快来咑总输好方法教你徽关注 AG 熊 猫</t>
+  </si>
+  <si>
+    <t>有在里面找  板奇  就知道了</t>
+  </si>
+  <si>
+    <t>西安 牛神 全瑛</t>
+  </si>
+  <si>
+    <t>西安牛神{8}全部英啊</t>
+  </si>
+  <si>
+    <t>西安牛 申 诠英</t>
+  </si>
+  <si>
+    <t>血徴狺  ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>观祝我，快乐女兵</t>
+  </si>
+  <si>
+    <t>访氺打鱼有诀窍，蚪晕扑才</t>
+  </si>
+  <si>
+    <t>访氺好捞，躲音扑才</t>
+  </si>
+  <si>
+    <t>住队 DCD 练YOU 稳稳待路</t>
+  </si>
+  <si>
+    <t>你们搜，满天文，拚写咖</t>
+  </si>
+  <si>
+    <t>免费陶消息好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>别搞错了 我徽??962?吃好</t>
+  </si>
+  <si>
+    <t>别搞错了徽??962?熊迪</t>
+  </si>
+  <si>
+    <t>劲団的DCD练起YOU</t>
+  </si>
+  <si>
+    <t>别搞错吃肉来徽??967?</t>
+  </si>
+  <si>
+    <t>劲団DCD抢红包YOU</t>
+  </si>
+  <si>
+    <t>完扑鱼看逗晕@管家鱼</t>
+  </si>
+  <si>
+    <t>快来咑总输好方法教你徽关注 AG 熊 猫</t>
+  </si>
+  <si>
+    <t>我今天收工了目标到位了你们呢 胃{65}关注A G博士</t>
+  </si>
+  <si>
+    <t>我要吃肉啊 ??353?这吗</t>
+  </si>
+  <si>
+    <t>来这里徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>来起飞徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>来搜v，如可哥，拼咖我</t>
+  </si>
+  <si>
+    <t>沛雪抱团啊 徴狺  ㄨ??774</t>
+  </si>
+  <si>
+    <t>没有套路闲暇来报徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>走内幕服气好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>走哈哈贷迎前pay连着后 nnd</t>
+  </si>
+  <si>
+    <t>那是你不会打吖教你徽关注 AG 熊 猫</t>
+  </si>
+  <si>
+    <t>到底怎么放氺卡鱼望躲英 席开名</t>
+  </si>
+  <si>
+    <t>到底怎么放氺卡鱼望躲英 古星华</t>
+  </si>
+  <si>
+    <t>剁暗@ 板罗  至波了</t>
+  </si>
+  <si>
+    <t>剁暗@ 花奇   有办法</t>
+  </si>
+  <si>
+    <t>鸡块DCD仔下YOU待</t>
+  </si>
+  <si>
+    <t>事DCD练起YOU转団</t>
+  </si>
+  <si>
+    <t>佺英{1}西安牛神</t>
+  </si>
+  <si>
+    <t>单总赚好方法教你徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>房间号徴狺  ?444 ?ㄨ</t>
+  </si>
+  <si>
+    <t>放水啦， 速来，蚪晕扑才</t>
+  </si>
+  <si>
+    <t>放水啦，速来蚪晕扑才</t>
+  </si>
+  <si>
+    <t>放氺鱼分看逗晕，管家鱼</t>
+  </si>
+  <si>
+    <t>放氺看逗晕，管家鱼</t>
+  </si>
+  <si>
+    <t>板面放水去打好捞，蚪晕乐才</t>
+  </si>
+  <si>
+    <t>沓，搜 米和哥 拚就行了</t>
+  </si>
+  <si>
+    <t>玩朵音@板罗  讲解达鱼了</t>
+  </si>
+  <si>
+    <t>玩朵音@花奇  看直播吧</t>
+  </si>
+  <si>
+    <t>玩鱼网逗晕@管家鱼，快乐扑鱼</t>
+  </si>
+  <si>
+    <t>玩鱼看朵晕@管家鱼</t>
+  </si>
+  <si>
+    <t>玩鱼逗晕@管家鱼，快乐扑鱼</t>
+  </si>
+  <si>
+    <t>玩鱼逗晕@管家鱼，解答</t>
+  </si>
+  <si>
+    <t>玩逗引@板罗 开播了</t>
+  </si>
+  <si>
+    <t>玩躲音@  板罗   奖解鱼办法</t>
+  </si>
+  <si>
+    <t>玩躲引@ 花奇  姜解半法</t>
+  </si>
+  <si>
+    <t>玩躲音@  花奇   开播列</t>
+  </si>
+  <si>
+    <t>玩躲音@ 乐 才  </t>
+  </si>
+  <si>
+    <t>玩躲音@ 板罗   开播了</t>
+  </si>
+  <si>
+    <t>玩躲音@ 乐才  开播了</t>
+  </si>
+  <si>
+    <t>玩躲音@ 板罗  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>玩躲音@ 花奇   直播了</t>
+  </si>
+  <si>
+    <t>玩躲音@板罗  讲节朴鱼法</t>
+  </si>
+  <si>
+    <t>玩躲音@板罗  奖解朴鱼法</t>
+  </si>
+  <si>
+    <t>玩躲音@板罗  開播咯</t>
+  </si>
+  <si>
+    <t>玩躲喑@  扑才  奖解鱼办法</t>
+  </si>
+  <si>
+    <t>玩躲喑@板罗  開播咯</t>
+  </si>
+  <si>
+    <t>盲目打不如遂美女大神徴狺 EOW?O?</t>
+  </si>
+  <si>
+    <t>盲目投注不如抓住转机徴狺  ㄨ??947</t>
+  </si>
+  <si>
+    <t>直录DCD练气YOU字幕袋赚</t>
+  </si>
+  <si>
+    <t>腾免费消息好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>腾内幕服气好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>稔出好路来好方法徽关注 AG大哥</t>
+  </si>
+  <si>
+    <t>睛内幕服气好方法徽关注 AG大哥</t>
+  </si>
+  <si>
+    <t>想赢钱搜，满天文，拚写咖</t>
+  </si>
+  <si>
+    <t>想知道瑛紋尋   吉林最強</t>
+  </si>
+  <si>
+    <t>想要団的DCD练起YOU</t>
+  </si>
+  <si>
+    <t>躲音@扑才，开播</t>
+  </si>
+  <si>
+    <t>躲音！特名义 开课之中</t>
+  </si>
+  <si>
+    <t>躲音 古星华 欢快濮渝中</t>
+  </si>
+  <si>
+    <t>躲音扑才，开播了</t>
+  </si>
+  <si>
+    <t>输钱没有方法了吗，蚪晕捕才开播</t>
+  </si>
+  <si>
+    <t>徴狺  ?444 ?ㄨ大师待赢钱不难</t>
+  </si>
+  <si>
+    <t>徴狺  ㄨ?ㄨ973上分就是这么简单</t>
+  </si>
+  <si>
+    <t>管家鱼是逗晕号看快乐扑鱼</t>
+  </si>
+  <si>
+    <t>裴雪儿讲座教你不上头原则 徴?  ㄨ?ㄨ973</t>
+  </si>
+  <si>
+    <t>嘿嘿哈是你不会教你徽关注 AG熊猫</t>
+  </si>
+  <si>
+    <t>潭内幕消息好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>線下瑛紋尋   吉林最強</t>
+  </si>
+  <si>
+    <t>線下瑛紋尋   吉林最強{88}</t>
+  </si>
+  <si>
+    <t>頞内幕消息好方法徽关注 AG名灯</t>
+  </si>
+  <si>
+    <t>學打鱼放水蚪晕扑才</t>
+  </si>
+  <si>
+    <t>薯片在下ㄨ??767</t>
+  </si>
+  <si>
+    <t>瞧好了关祝，快乐女兵</t>
+  </si>
+  <si>
+    <t>徽 吃肉来??962?</t>
+  </si>
+  <si>
+    <t>徽呢 ??755?{84}</t>
+  </si>
+  <si>
+    <t>徽徽嫁好??735?</t>
+  </si>
+  <si>
+    <t>徽??962?没空格</t>
+  </si>
+  <si>
+    <t>還不會怎么打吗，蚪晕捕才，开播了</t>
+  </si>
+  <si>
+    <t>還不會怎么玩的蚪晕扑才</t>
+  </si>
+  <si>
+    <t>赣出好路来好方法徽关注 AG大哥</t>
+  </si>
+  <si>
+    <t>玩躲喑@  板罗  开播列</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲喑</t>
+  </si>
+  <si>
+    <t>趣玩躲喑</t>
+  </si>
+  <si>
+    <t>花奇</t>
+  </si>
+  <si>
+    <t>板罗</t>
+  </si>
+  <si>
+    <t>板罗  开播</t>
+  </si>
+  <si>
+    <t>开播</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>躲喑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>管家鱼</t>
+  </si>
+  <si>
+    <t>躲晕号</t>
+  </si>
+  <si>
+    <t>无空格</t>
+  </si>
+  <si>
+    <t>空格</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>qwe无空格xxx</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲音@</t>
+  </si>
+  <si>
+    <t>上分卡鱼</t>
+  </si>
+  <si>
+    <t>连着啊</t>
+  </si>
+  <si>
+    <t>财神送</t>
+  </si>
+  <si>
+    <t>财神送金</t>
+  </si>
+  <si>
+    <t>躲音</t>
+  </si>
+  <si>
+    <t> 管家鱼</t>
+  </si>
+  <si>
+    <t>徴狺</t>
+  </si>
+  <si>
+    <t>上分徴狺</t>
+  </si>
+  <si>
+    <t>赢钱不难</t>
+  </si>
+  <si>
+    <t>A G博士</t>
+  </si>
+  <si>
+    <t>关注A G博士</t>
+  </si>
+  <si>
+    <t>关注</t>
+  </si>
+  <si>
+    <t>徽关注 AG大姐姐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>语纹 扌并</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拚写咖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>你们搜，满天文，拚写咖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>满天文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>徽关注 AG 熊 猫</t>
+  </si>
+  <si>
+    <t>徽关注</t>
+  </si>
+  <si>
+    <t>徽关注</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲音</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲音乐才</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲喑@  扑才</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扑才</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲音@ 花奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>玩躲音@ 板罗</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>盲目打不如遂美女大神徴狺 EOW?O?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>美女大神徴狺</t>
+  </si>
+  <si>
+    <t>好方法徽关注</t>
+  </si>
+  <si>
+    <t>名灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AG名灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>瑛紋尋</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>懂得趣玩躲喑</t>
+  </si>
+  <si>
+    <t>懂得趣玩躲喑花奇</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖解鱼办法</t>
+  </si>
+  <si>
+    <t>徽没空格</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -579,7 +1253,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -611,6 +1285,13 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -629,15 +1310,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -657,9 +1339,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="2" xr:uid="{BE10E4D1-4FCA-4955-9B38-4FB46049060D}"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -938,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B171"/>
+  <dimension ref="A1:B396"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A179" sqref="A179"/>
+    <sheetView tabSelected="1" topLeftCell="A385" workbookViewId="0">
+      <selection activeCell="D401" sqref="D401"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2317,10 +3006,1816 @@
         <v>0</v>
       </c>
     </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="B179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="B180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="B181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B185">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="B186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A204" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="B204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A205" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="B205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A206" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="B206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A207" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A208" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A209" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A210" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A211" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A212" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A213" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="B213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A214" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A215" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A216" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A217" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A218" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A219" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B219">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A220" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A221" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A222" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="B222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A223" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="B223">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A224" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A225" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A226" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A227" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A228" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="B228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A229" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A230" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="B230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A231" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B231">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A232" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A233" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B233">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A234" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A235" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A236" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A237" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="B237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A238" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A239" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="B239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A240" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A241" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A242" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A243" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="B243">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A244" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A245" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="B245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A246" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A247" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="B247">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A248" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="B248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A249" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="B249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A250" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A251" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A252" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="B252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A253" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B253">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A254" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="B254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A255" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="B255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A256" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="B256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A257" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="B257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A258" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="B258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A259" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="B259">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A260" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="B260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A261" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="B261">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A262" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="B262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A263" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="B263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A264" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="B264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A265" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="B266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="B267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="B269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="B270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="B272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="B273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="B275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="B280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="B282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="B287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="B293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="B295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A302" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A303" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A304" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A305" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B305">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A306" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A307" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="B307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A308" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A309" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A310" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="B310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A311" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A312" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A313" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="B313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A314" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A315" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="B315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A316" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A317" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A318" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A319" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="B319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="B321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="B325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B326">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="B327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="B331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B332">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="B333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="B335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A337" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A338" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="B338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A339" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A340" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="B340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A341" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A342" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="B342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A343" t="s">
+        <v>333</v>
+      </c>
+      <c r="B343">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>334</v>
+      </c>
+      <c r="B344">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>335</v>
+      </c>
+      <c r="B345">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>336</v>
+      </c>
+      <c r="B346">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>337</v>
+      </c>
+      <c r="B347">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>338</v>
+      </c>
+      <c r="B348">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>333</v>
+      </c>
+      <c r="B349">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>339</v>
+      </c>
+      <c r="B350">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>340</v>
+      </c>
+      <c r="B351">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>341</v>
+      </c>
+      <c r="B352">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>342</v>
+      </c>
+      <c r="B353">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>343</v>
+      </c>
+      <c r="B354">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B355">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>345</v>
+      </c>
+      <c r="B356">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>346</v>
+      </c>
+      <c r="B357">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>347</v>
+      </c>
+      <c r="B358">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>348</v>
+      </c>
+      <c r="B359">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>349</v>
+      </c>
+      <c r="B360">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>350</v>
+      </c>
+      <c r="B361">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>351</v>
+      </c>
+      <c r="B362">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>352</v>
+      </c>
+      <c r="B363">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>353</v>
+      </c>
+      <c r="B364">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>354</v>
+      </c>
+      <c r="B365">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>355</v>
+      </c>
+      <c r="B366">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>356</v>
+      </c>
+      <c r="B367">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>357</v>
+      </c>
+      <c r="B368">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A369" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B369">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A370" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B370">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A371" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B371">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A372" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="B372">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A373" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B373">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A374" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B374">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>363</v>
+      </c>
+      <c r="B375">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A376" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B376">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>366</v>
+      </c>
+      <c r="B377">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A378" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B378">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A379" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B379">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A380" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B380">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A381" s="8" t="s">
+        <v>368</v>
+      </c>
+      <c r="B381">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>369</v>
+      </c>
+      <c r="B382">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>335</v>
+      </c>
+      <c r="B383">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>336</v>
+      </c>
+      <c r="B384">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A385" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B385">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>373</v>
+      </c>
+      <c r="B386">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>374</v>
+      </c>
+      <c r="B387">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>376</v>
+      </c>
+      <c r="B388">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>375</v>
+      </c>
+      <c r="B389">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>377</v>
+      </c>
+      <c r="B390">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>378</v>
+      </c>
+      <c r="B391">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>379</v>
+      </c>
+      <c r="B392">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>380</v>
+      </c>
+      <c r="B393">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>328</v>
+      </c>
+      <c r="B394">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>381</v>
+      </c>
+      <c r="B395">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>364</v>
+      </c>
+      <c r="B396">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{9007686D-7565-4E50-BF8F-1EB4B9B99C50}"/>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A175" r:id="rId1" xr:uid="{3B37F06C-6F9B-4765-A9A8-B97A4A4D5F1B}"/>
+    <hyperlink ref="A381" r:id="rId2" xr:uid="{A7D0676E-A9C0-49F9-A97A-F1E1A2A58487}"/>
+    <hyperlink ref="A380" r:id="rId3" xr:uid="{EEE6950F-3CAE-43AC-88A7-8A8ED3D8A3FB}"/>
+    <hyperlink ref="A379" r:id="rId4" xr:uid="{2F503338-110D-4200-BFDD-CA43C5BFE28C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v1.2.3 add new word in excel
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/chat_content_20200512.xlsx
+++ b/ai/assets/textbook/chat_content_20200512.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2230C46-27DF-4606-9C31-E76B591A439E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1782FD56-4A83-4486-B247-0ED831FF1E72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29580" yWindow="2040" windowWidth="21105" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="870" yWindow="735" windowWidth="27390" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="374">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="376">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1233,6 +1233,12 @@
   <si>
     <t>在的</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完朵因@ 板罗 呐里早</t>
+  </si>
+  <si>
+    <t>玩躲阴@  罗奇  呐里有</t>
   </si>
 </sst>
 </file>
@@ -1613,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B389"/>
+  <dimension ref="A1:B391"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
-      <selection activeCell="A394" sqref="A394"/>
+    <sheetView tabSelected="1" topLeftCell="A376" workbookViewId="0">
+      <selection activeCell="H395" sqref="H395"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -4734,6 +4740,22 @@
       </c>
       <c r="B389">
         <v>0</v>
+      </c>
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>374</v>
+      </c>
+      <c r="B390">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>375</v>
+      </c>
+      <c r="B391">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tmp save for 1.2.7
</commit_message>
<xml_diff>
--- a/ai/assets/textbook/chat_content_20200512.xlsx
+++ b/ai/assets/textbook/chat_content_20200512.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AIChatFilter\service\ai-chatfilter-service\ai\assets\textbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8C00257-FA71-4D8A-A9D1-B70A49102DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A903C831-F3CD-44D2-B372-845803F0D490}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="870" windowWidth="27390" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30210" yWindow="3120" windowWidth="27390" windowHeight="11850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$B$329</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="316">
   <si>
     <t>发言内容</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -152,9 +152,6 @@
     <t>听想赢钱就来徽关注公丛 AG山哥 教你赢不收钱</t>
   </si>
   <si>
-    <t>{viplv0}{dt1-10-5-28}你家死光了啊</t>
-  </si>
-  <si>
     <t>{viplv0}{dt1-10-6-23}真特么恶心</t>
   </si>
   <si>
@@ -197,9 +194,6 @@
     <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-11-6-29&lt;/dt&gt;真她妈&lt;isAnchorPlatformMsg&gt;0&lt;/isAnchorPlatformMs</t>
   </si>
   <si>
-    <t>&lt;msg&gt;&lt;yplv&gt;6&lt;/yplv&gt;&lt;prm&gt;1&lt;/prm&gt;&lt;dt&gt;1-0-5-30&lt;/dt&gt;我刚才就是用的V搜的&lt;isAnchorPlatformMsg&gt;0&lt;/</t>
-  </si>
-  <si>
     <t>tnnd</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>乧暗秒杀鱼</t>
   </si>
   <si>
-    <t>车牌 ????163??</t>
-  </si>
-  <si>
     <t>加它吗后台老板</t>
   </si>
   <si>
@@ -266,9 +257,6 @@
     <t>别急，日死她们</t>
   </si>
   <si>
-    <t>我翻车牌 ????163??</t>
-  </si>
-  <si>
     <t>車隊躺好 瑛纹尋 美丽上海</t>
   </si>
   <si>
@@ -386,9 +374,6 @@
     <t>输钱蚪晕特名华</t>
   </si>
   <si>
-    <t>随我的车牌 ????163??</t>
-  </si>
-  <si>
     <t>赚我的钱不公道死係全家</t>
   </si>
   <si>
@@ -399,12 +384,6 @@
   </si>
   <si>
     <t>澳门海哥&lt;迷途的请来非诚勿扰</t>
-  </si>
-  <si>
-    <t>懂得规划才能赢利????163??</t>
-  </si>
-  <si>
-    <t>是车牌 ????163??</t>
   </si>
   <si>
     <t>魅力上海  瑛纹尋  早班车</t>
@@ -467,9 +446,6 @@
     <t>玩躲喑@  板罗  奖解鱼办法</t>
   </si>
   <si>
-    <t>666上分卡鱼就系躲晕号   管家鱼</t>
-  </si>
-  <si>
     <t>bye无空格yao{77}</t>
   </si>
   <si>
@@ -506,27 +482,9 @@
     <t>two前面的off后面</t>
   </si>
   <si>
-    <t>v,如可哥，拼，都懂的</t>
-  </si>
-  <si>
     <t>XBB视讯</t>
   </si>
   <si>
-    <t>ㄨ??767薯片</t>
-  </si>
-  <si>
-    <t>ㄨ?ㄨ973</t>
-  </si>
-  <si>
-    <t>ㄨ??356</t>
-  </si>
-  <si>
-    <t>ㄨ??168</t>
-  </si>
-  <si>
-    <t>ㄨ??552</t>
-  </si>
-  <si>
     <t>人人都有机会看你抓不抓得住了徴狺  ㄨ??947</t>
   </si>
   <si>
@@ -539,18 +497,6 @@
     <t>上分卡鱼就系躲晕号   管家鱼</t>
   </si>
   <si>
-    <t>上分回复徴狺  ㄨ??947</t>
-  </si>
-  <si>
-    <t>上分徴狺  ㄨ??947</t>
-  </si>
-  <si>
-    <t>上暗??????</t>
-  </si>
-  <si>
-    <t>上暗躺赢徽??????</t>
-  </si>
-  <si>
     <t>大师待赢钱不难徴狺  ?444 ?ㄨ机会不要错过</t>
   </si>
   <si>
@@ -632,18 +578,6 @@
     <t>吃肉会会徽??967?抓图吃</t>
   </si>
   <si>
-    <t>吃肉的??353?{89}</t>
-  </si>
-  <si>
-    <t>吃肉家会??962? 吃肉</t>
-  </si>
-  <si>
-    <t>吃肉随我 ??981?</t>
-  </si>
-  <si>
-    <t>吃香香徽??962?</t>
-  </si>
-  <si>
     <t>妇内幕消息好方法徽关注 AG名灯</t>
   </si>
   <si>
@@ -665,9 +599,6 @@
     <t>西安牛 申 诠英</t>
   </si>
   <si>
-    <t>血徴狺  ㄨ?ㄨ973</t>
-  </si>
-  <si>
     <t>访氺打鱼有诀窍，蚪晕扑才</t>
   </si>
   <si>
@@ -683,18 +614,9 @@
     <t>免费陶消息好方法徽关注 AG名灯</t>
   </si>
   <si>
-    <t>别搞错了 我徽??962?吃好</t>
-  </si>
-  <si>
-    <t>别搞错了徽??962?熊迪</t>
-  </si>
-  <si>
     <t>劲団的DCD练起YOU</t>
   </si>
   <si>
-    <t>别搞错吃肉来徽??967?</t>
-  </si>
-  <si>
     <t>劲団DCD抢红包YOU</t>
   </si>
   <si>
@@ -707,24 +629,9 @@
     <t>我今天收工了目标到位了你们呢 胃{65}关注A G博士</t>
   </si>
   <si>
-    <t>我要吃肉啊 ??353?这吗</t>
-  </si>
-  <si>
-    <t>来这里徴狺  ㄨ??947</t>
-  </si>
-  <si>
-    <t>来起飞徴狺  ㄨ??947</t>
-  </si>
-  <si>
     <t>来搜v，如可哥，拼咖我</t>
   </si>
   <si>
-    <t>沛雪抱团啊 徴狺  ㄨ??774</t>
-  </si>
-  <si>
-    <t>没有套路闲暇来报徴狺  ㄨ??947</t>
-  </si>
-  <si>
     <t>走内幕服气好方法徽关注 AG名灯</t>
   </si>
   <si>
@@ -875,15 +782,9 @@
     <t>徴狺  ?444 ?ㄨ大师待赢钱不难</t>
   </si>
   <si>
-    <t>徴狺  ㄨ?ㄨ973上分就是这么简单</t>
-  </si>
-  <si>
     <t>管家鱼是逗晕号看快乐扑鱼</t>
   </si>
   <si>
-    <t>裴雪儿讲座教你不上头原则 徴?  ㄨ?ㄨ973</t>
-  </si>
-  <si>
     <t>嘿嘿哈是你不会教你徽关注 AG熊猫</t>
   </si>
   <si>
@@ -903,15 +804,6 @@
   </si>
   <si>
     <t>瞧好了关祝，快乐女兵</t>
-  </si>
-  <si>
-    <t>徽 吃肉来??962?</t>
-  </si>
-  <si>
-    <t>徽呢 ??755?{84}</t>
-  </si>
-  <si>
-    <t>徽徽嫁好??735?</t>
   </si>
   <si>
     <t>徽??962?没空格</t>
@@ -1144,6 +1036,17 @@
   <si>
     <t>剁暗@ 板罗  至波了</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{viplv0}{dt1-10-5-28}你家死光了啊</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v,如可哥，拼，都懂的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>都懂的</t>
   </si>
 </sst>
 </file>
@@ -1524,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B364"/>
+  <dimension ref="A1:B329"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="A217" sqref="A217"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1777,7 +1680,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>32</v>
+        <v>313</v>
       </c>
       <c r="B31">
         <v>4</v>
@@ -1785,7 +1688,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32">
         <v>4</v>
@@ -1793,7 +1696,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33">
         <v>4</v>
@@ -1801,7 +1704,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34">
         <v>4</v>
@@ -1809,7 +1712,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35">
         <v>4</v>
@@ -1817,7 +1720,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36">
         <v>4</v>
@@ -1825,7 +1728,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37">
         <v>4</v>
@@ -1833,7 +1736,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38">
         <v>4</v>
@@ -1841,7 +1744,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -1849,7 +1752,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>4</v>
@@ -1857,7 +1760,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41">
         <v>4</v>
@@ -1865,7 +1768,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42">
         <v>4</v>
@@ -1873,7 +1776,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B43">
         <v>4</v>
@@ -1881,7 +1784,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B44">
         <v>4</v>
@@ -1889,31 +1792,31 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="B46">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B48">
         <v>1</v>
@@ -1921,7 +1824,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1929,31 +1832,31 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="B52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="B52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1961,23 +1864,23 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="B55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1985,15 +1888,15 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="B57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -2001,7 +1904,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -2009,15 +1912,15 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -2025,15 +1928,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="B62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -2041,7 +1944,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -2049,7 +1952,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -2057,7 +1960,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -2065,31 +1968,31 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="B68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="B69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="B69">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -2097,7 +2000,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B71">
         <v>1</v>
@@ -2105,7 +2008,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -2113,7 +2016,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -2121,7 +2024,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -2129,7 +2032,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -2137,7 +2040,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B76">
         <v>1</v>
@@ -2145,15 +2048,15 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="B78">
         <v>1</v>
@@ -2161,15 +2064,15 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="B79">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -2177,23 +2080,23 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="B82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="B82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>84</v>
       </c>
       <c r="B83">
         <v>1</v>
@@ -2201,7 +2104,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -2209,15 +2112,15 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="B85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="B86">
         <v>1</v>
@@ -2225,79 +2128,79 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
+      <c r="B88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B88">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="B89">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="B92">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B93">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B94">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
+      <c r="B95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="B95">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="B96">
         <v>1</v>
@@ -2305,15 +2208,15 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="B98">
         <v>1</v>
@@ -2321,7 +2224,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -2329,31 +2232,31 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
+      <c r="B102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="B101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="B102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="B103">
         <v>1</v>
@@ -2368,32 +2271,32 @@
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="3" t="s">
+      <c r="A105" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
+      <c r="B106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="B106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -2401,7 +2304,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -2409,23 +2312,23 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="B110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2433,23 +2336,23 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
+      <c r="B114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A115" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="B114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="2" t="s">
-        <v>114</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -2457,55 +2360,55 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A118" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="B116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="B117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="B118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B119">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="B120">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="B121">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="B122">
         <v>1</v>
@@ -2513,50 +2416,50 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B123">
         <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="3" t="s">
-        <v>27</v>
+      <c r="A124" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="B124">
         <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="4" t="s">
-        <v>28</v>
+      <c r="A125" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="B125">
         <v>1</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>29</v>
+      <c r="A126" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="B126">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>30</v>
+      <c r="A127" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>31</v>
+        <v>121</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2564,19 +2467,19 @@
         <v>122</v>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="6" t="s">
         <v>123</v>
       </c>
       <c r="B130">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B131">
@@ -2584,7 +2487,7 @@
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="7" t="s">
         <v>125</v>
       </c>
       <c r="B132">
@@ -2592,48 +2495,48 @@
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="7" t="s">
         <v>126</v>
       </c>
       <c r="B133">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="B134">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="2" t="s">
+      <c r="B135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B135">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
+      <c r="B136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B136">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="6" t="s">
-        <v>130</v>
-      </c>
       <c r="B137">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B138">
         <v>1</v>
@@ -2641,7 +2544,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2649,15 +2552,15 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" s="7" t="s">
         <v>133</v>
-      </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="4" t="s">
-        <v>287</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2705,7 +2608,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>139</v>
+        <v>315</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2713,7 +2616,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
-        <v>140</v>
+        <v>314</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -2721,7 +2624,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -2729,7 +2632,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -2737,7 +2640,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2745,7 +2648,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B152">
         <v>1</v>
@@ -2753,7 +2656,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -2761,7 +2664,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B154">
         <v>1</v>
@@ -2769,7 +2672,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -2777,7 +2680,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -2785,7 +2688,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -2793,7 +2696,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B158">
         <v>1</v>
@@ -2801,7 +2704,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -2809,7 +2712,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B160">
         <v>1</v>
@@ -2817,7 +2720,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -2825,7 +2728,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B162">
         <v>1</v>
@@ -2833,7 +2736,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -2841,7 +2744,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -2849,7 +2752,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -2857,7 +2760,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -2865,7 +2768,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -2873,7 +2776,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B168">
         <v>1</v>
@@ -2881,7 +2784,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -2889,7 +2792,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -2897,7 +2800,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -2905,7 +2808,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B172">
         <v>1</v>
@@ -2913,7 +2816,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -2921,7 +2824,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B174">
         <v>1</v>
@@ -2929,7 +2832,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -2937,7 +2840,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B176">
         <v>1</v>
@@ -2945,7 +2848,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -2953,7 +2856,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B178">
         <v>1</v>
@@ -2961,7 +2864,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -2969,7 +2872,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B180">
         <v>1</v>
@@ -2977,7 +2880,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -2985,7 +2888,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B182">
         <v>1</v>
@@ -2993,7 +2896,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -3001,7 +2904,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -3009,7 +2912,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -3017,7 +2920,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" s="7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -3025,7 +2928,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -3033,7 +2936,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B188">
         <v>1</v>
@@ -3041,7 +2944,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -3049,7 +2952,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B190">
         <v>1</v>
@@ -3057,7 +2960,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -3065,7 +2968,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B192">
         <v>1</v>
@@ -3073,7 +2976,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -3081,7 +2984,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B194">
         <v>1</v>
@@ -3089,7 +2992,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -3097,7 +3000,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B196">
         <v>1</v>
@@ -3105,7 +3008,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -3113,7 +3016,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B198">
         <v>1</v>
@@ -3121,7 +3024,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -3129,7 +3032,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B200">
         <v>1</v>
@@ -3137,7 +3040,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -3145,7 +3048,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B202">
         <v>1</v>
@@ -3153,15 +3056,15 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B203">
         <v>1</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A204" s="7" t="s">
-        <v>196</v>
+      <c r="A204" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="B204">
         <v>1</v>
@@ -3169,7 +3072,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A205" s="7" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -3177,7 +3080,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A206" s="7" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="B206">
         <v>1</v>
@@ -3185,7 +3088,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A207" s="7" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -3193,7 +3096,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A208" s="7" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B208">
         <v>1</v>
@@ -3201,7 +3104,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A209" s="7" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -3209,7 +3112,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A210" s="7" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B210">
         <v>1</v>
@@ -3217,7 +3120,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A211" s="7" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -3225,7 +3128,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A212" s="7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="B212">
         <v>1</v>
@@ -3233,7 +3136,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A213" s="7" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -3241,7 +3144,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A214" s="7" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B214">
         <v>1</v>
@@ -3249,7 +3152,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A215" s="7" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="B215">
         <v>1</v>
@@ -3257,7 +3160,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A216" s="7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B216">
         <v>1</v>
@@ -3265,7 +3168,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A217" s="7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -3273,7 +3176,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A218" s="7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B218">
         <v>1</v>
@@ -3281,7 +3184,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -3289,7 +3192,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A220" s="7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="B220">
         <v>1</v>
@@ -3297,7 +3200,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A221" s="7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -3305,7 +3208,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A222" s="7" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B222">
         <v>1</v>
@@ -3313,7 +3216,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A223" s="7" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -3321,7 +3224,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A224" s="7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B224">
         <v>1</v>
@@ -3329,7 +3232,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A225" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -3337,7 +3240,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A226" s="7" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B226">
         <v>1</v>
@@ -3345,7 +3248,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A227" s="7" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -3353,7 +3256,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A228" s="7" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B228">
         <v>1</v>
@@ -3361,7 +3264,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A229" s="7" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -3369,7 +3272,7 @@
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A230" s="7" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B230">
         <v>1</v>
@@ -3377,7 +3280,7 @@
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A231" s="7" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B231">
         <v>1</v>
@@ -3385,15 +3288,15 @@
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A232" s="7" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B232">
         <v>1</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A233" s="4" t="s">
-        <v>348</v>
+      <c r="A233" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="B233">
         <v>1</v>
@@ -3401,7 +3304,7 @@
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A234" s="7" t="s">
-        <v>225</v>
+        <v>126</v>
       </c>
       <c r="B234">
         <v>1</v>
@@ -3409,7 +3312,7 @@
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A235" s="7" t="s">
-        <v>226</v>
+        <v>125</v>
       </c>
       <c r="B235">
         <v>1</v>
@@ -3417,7 +3320,7 @@
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A236" s="7" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="B236">
         <v>1</v>
@@ -3425,7 +3328,7 @@
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A237" s="7" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -3433,7 +3336,7 @@
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A238" s="7" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B238">
         <v>1</v>
@@ -3441,7 +3344,7 @@
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A239" s="7" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -3449,7 +3352,7 @@
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A240" s="7" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B240">
         <v>1</v>
@@ -3457,7 +3360,7 @@
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A241" s="7" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -3465,7 +3368,7 @@
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A242" s="7" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B242">
         <v>1</v>
@@ -3473,7 +3376,7 @@
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A243" s="7" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -3481,7 +3384,7 @@
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A244" s="7" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B244">
         <v>1</v>
@@ -3489,7 +3392,7 @@
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A245" s="7" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="B245">
         <v>1</v>
@@ -3497,7 +3400,7 @@
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A246" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B246">
         <v>1</v>
@@ -3505,7 +3408,7 @@
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A247" s="7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -3513,7 +3416,7 @@
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A248" s="7" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="B248">
         <v>1</v>
@@ -3521,7 +3424,7 @@
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A249" s="7" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -3529,7 +3432,7 @@
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A250" s="7" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="B250">
         <v>1</v>
@@ -3537,7 +3440,7 @@
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A251" s="7" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -3545,7 +3448,7 @@
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A252" s="7" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B252">
         <v>1</v>
@@ -3553,7 +3456,7 @@
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A253" s="7" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -3561,7 +3464,7 @@
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A254" s="7" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B254">
         <v>1</v>
@@ -3569,7 +3472,7 @@
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -3577,7 +3480,7 @@
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A256" s="7" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="B256">
         <v>1</v>
@@ -3585,7 +3488,7 @@
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A257" s="7" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -3593,7 +3496,7 @@
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A258" s="7" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B258">
         <v>1</v>
@@ -3601,7 +3504,7 @@
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A259" s="7" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -3609,7 +3512,7 @@
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A260" s="7" t="s">
-        <v>251</v>
+        <v>124</v>
       </c>
       <c r="B260">
         <v>1</v>
@@ -3617,7 +3520,7 @@
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A261" s="7" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -3625,7 +3528,7 @@
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A262" s="7" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B262">
         <v>1</v>
@@ -3633,311 +3536,311 @@
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>133</v>
+        <v>250</v>
       </c>
       <c r="B263">
         <v>1</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A264" s="7" t="s">
-        <v>132</v>
+      <c r="A264" t="s">
+        <v>252</v>
       </c>
       <c r="B264">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A265" s="7" t="s">
+      <c r="A265" t="s">
+        <v>253</v>
+      </c>
+      <c r="B265">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A266" t="s">
         <v>254</v>
       </c>
-      <c r="B265">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A266" s="7" t="s">
+      <c r="B266">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
         <v>255</v>
       </c>
-      <c r="B266">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A267" s="7" t="s">
+      <c r="B267">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A268" t="s">
         <v>256</v>
       </c>
-      <c r="B267">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A268" s="7" t="s">
+      <c r="B268">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
         <v>257</v>
       </c>
-      <c r="B268">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A269" s="7" t="s">
+      <c r="B269">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A270" t="s">
+        <v>252</v>
+      </c>
+      <c r="B270">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
         <v>258</v>
       </c>
-      <c r="B269">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A270" s="7" t="s">
+      <c r="B271">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A272" t="s">
         <v>259</v>
       </c>
-      <c r="B270">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A271" s="7" t="s">
+      <c r="B272">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
         <v>260</v>
       </c>
-      <c r="B271">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A272" s="7" t="s">
+      <c r="B273">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A274" t="s">
         <v>261</v>
       </c>
-      <c r="B272">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="273" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A273" s="7" t="s">
+      <c r="B274">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
         <v>262</v>
       </c>
-      <c r="B273">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A274" s="7" t="s">
+      <c r="B275">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A276" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B274">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="275" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A275" s="7" t="s">
+      <c r="B276">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
         <v>264</v>
       </c>
-      <c r="B275">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A276" s="7" t="s">
+      <c r="B277">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A278" t="s">
         <v>265</v>
       </c>
-      <c r="B276">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A277" s="7" t="s">
+      <c r="B278">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
         <v>266</v>
       </c>
-      <c r="B277">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="278" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A278" s="7" t="s">
+      <c r="B279">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A280" t="s">
         <v>267</v>
       </c>
-      <c r="B278">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="279" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A279" s="7" t="s">
+      <c r="B280">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
         <v>268</v>
       </c>
-      <c r="B279">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="280" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A280" s="7" t="s">
+      <c r="B281">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A282" t="s">
         <v>269</v>
       </c>
-      <c r="B280">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="281" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A281" s="7" t="s">
+      <c r="B282">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
         <v>270</v>
       </c>
-      <c r="B281">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="282" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A282" s="7" t="s">
+      <c r="B283">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A284" t="s">
         <v>271</v>
       </c>
-      <c r="B282">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="283" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A283" s="7" t="s">
+      <c r="B284">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
         <v>272</v>
       </c>
-      <c r="B283">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="284" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A284" s="7" t="s">
+      <c r="B285">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A286" t="s">
         <v>273</v>
       </c>
-      <c r="B284">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="285" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A285" s="7" t="s">
+      <c r="B286">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
         <v>274</v>
       </c>
-      <c r="B285">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="286" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A286" s="7" t="s">
+      <c r="B287">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A288" t="s">
         <v>275</v>
       </c>
-      <c r="B286">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="287" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A287" s="7" t="s">
+      <c r="B288">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A289" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B289">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A290" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="B287">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="288" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A288" s="7" t="s">
+      <c r="B290">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A291" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="B288">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="289" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A289" s="7" t="s">
+      <c r="B291">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A292" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="B292">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A293" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="B289">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="290" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A290" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="B290">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="291" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A291" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B291">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="292" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A292" s="7" t="s">
+      <c r="B293">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A294" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="B292">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="293" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A293" s="7" t="s">
+      <c r="B294">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
         <v>281</v>
       </c>
-      <c r="B293">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="294" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A294" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="B294">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="295" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A295" s="7" t="s">
+      <c r="B295">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A296" s="2" t="s">
         <v>283</v>
       </c>
-      <c r="B295">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="296" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A296" s="7" t="s">
+      <c r="B296">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
         <v>284</v>
       </c>
-      <c r="B296">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="297" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A297" s="7" t="s">
+      <c r="B297">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A298" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="B297">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="298" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A298" s="7" t="s">
+      <c r="B298">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A299" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B299">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A300" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B300">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A301" s="8" t="s">
         <v>286</v>
-      </c>
-      <c r="B298">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="299" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A299" t="s">
-        <v>288</v>
-      </c>
-      <c r="B299">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="300" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A300" t="s">
-        <v>289</v>
-      </c>
-      <c r="B300">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="301" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A301" t="s">
-        <v>290</v>
       </c>
       <c r="B301">
         <v>4</v>
@@ -3945,7 +3848,7 @@
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B302">
         <v>4</v>
@@ -3953,7 +3856,7 @@
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>292</v>
+        <v>254</v>
       </c>
       <c r="B303">
         <v>4</v>
@@ -3961,15 +3864,15 @@
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>293</v>
+        <v>255</v>
       </c>
       <c r="B304">
         <v>4</v>
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A305" t="s">
-        <v>288</v>
+      <c r="A305" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="B305">
         <v>4</v>
@@ -3977,7 +3880,7 @@
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B306">
         <v>4</v>
@@ -3985,7 +3888,7 @@
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="B307">
         <v>4</v>
@@ -3993,7 +3896,7 @@
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B308">
         <v>4</v>
@@ -4001,7 +3904,7 @@
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B309">
         <v>4</v>
@@ -4009,15 +3912,15 @@
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="B310">
         <v>4</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A311" s="2" t="s">
-        <v>299</v>
+      <c r="A311" t="s">
+        <v>296</v>
       </c>
       <c r="B311">
         <v>4</v>
@@ -4025,7 +3928,7 @@
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B312">
         <v>4</v>
@@ -4033,7 +3936,7 @@
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="B313">
         <v>4</v>
@@ -4041,7 +3944,7 @@
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>302</v>
+        <v>247</v>
       </c>
       <c r="B314">
         <v>4</v>
@@ -4049,7 +3952,7 @@
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B315">
         <v>4</v>
@@ -4057,7 +3960,7 @@
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>304</v>
+        <v>282</v>
       </c>
       <c r="B316">
         <v>4</v>
@@ -4065,397 +3968,117 @@
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B317">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="B318">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="B319">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>308</v>
+        <v>123</v>
       </c>
       <c r="B320">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="B321">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="B322">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
+        <v>305</v>
+      </c>
+      <c r="B323">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>306</v>
+      </c>
+      <c r="B324">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>307</v>
+      </c>
+      <c r="B325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>308</v>
+      </c>
+      <c r="B326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>309</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>310</v>
+      </c>
+      <c r="B328">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
         <v>311</v>
       </c>
-      <c r="B323">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A324" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="B324">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A325" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B325">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A326" s="2" t="s">
-        <v>313</v>
-      </c>
-      <c r="B326">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A327" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B327">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A328" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B328">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A329" s="2" t="s">
-        <v>316</v>
-      </c>
       <c r="B329">
         <v>4</v>
       </c>
     </row>
-    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A330" t="s">
-        <v>317</v>
-      </c>
-      <c r="B330">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A331" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="B331">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A332" t="s">
-        <v>320</v>
-      </c>
-      <c r="B332">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A333" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="B333">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A334" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="B334">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A335" s="8" t="s">
-        <v>324</v>
-      </c>
-      <c r="B335">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A336" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B336">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="337" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A337" t="s">
-        <v>323</v>
-      </c>
-      <c r="B337">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="338" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A338" t="s">
-        <v>290</v>
-      </c>
-      <c r="B338">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="339" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A339" t="s">
-        <v>291</v>
-      </c>
-      <c r="B339">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="340" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A340" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="B340">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="341" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A341" t="s">
-        <v>327</v>
-      </c>
-      <c r="B341">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="342" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A342" t="s">
-        <v>328</v>
-      </c>
-      <c r="B342">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="343" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A343" t="s">
-        <v>330</v>
-      </c>
-      <c r="B343">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="344" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A344" t="s">
-        <v>329</v>
-      </c>
-      <c r="B344">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="345" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A345" t="s">
-        <v>331</v>
-      </c>
-      <c r="B345">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="346" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A346" t="s">
-        <v>332</v>
-      </c>
-      <c r="B346">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="347" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>333</v>
-      </c>
-      <c r="B347">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="348" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>334</v>
-      </c>
-      <c r="B348">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" t="s">
-        <v>283</v>
-      </c>
-      <c r="B349">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>335</v>
-      </c>
-      <c r="B350">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A351" t="s">
-        <v>318</v>
-      </c>
-      <c r="B351">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A352" t="s">
-        <v>336</v>
-      </c>
-      <c r="B352">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A353" t="s">
-        <v>337</v>
-      </c>
-      <c r="B353">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A354" t="s">
-        <v>338</v>
-      </c>
-      <c r="B354">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A355" t="s">
-        <v>130</v>
-      </c>
-      <c r="B355">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A356" t="s">
-        <v>339</v>
-      </c>
-      <c r="B356">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A357" t="s">
-        <v>340</v>
-      </c>
-      <c r="B357">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A358" t="s">
-        <v>341</v>
-      </c>
-      <c r="B358">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="359" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A359" t="s">
-        <v>342</v>
-      </c>
-      <c r="B359">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="360" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A360" t="s">
-        <v>343</v>
-      </c>
-      <c r="B360">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="361" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A361" t="s">
-        <v>344</v>
-      </c>
-      <c r="B361">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="362" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>345</v>
-      </c>
-      <c r="B362">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="363" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>346</v>
-      </c>
-      <c r="B363">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="364" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A364" t="s">
-        <v>347</v>
-      </c>
-      <c r="B364">
-        <v>4</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:B1" xr:uid="{9007686D-7565-4E50-BF8F-1EB4B9B99C50}"/>
+  <autoFilter ref="A1:B329" xr:uid="{C1ED4521-20B8-474E-B6CA-0E1178B0167B}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A141" r:id="rId1" xr:uid="{3B37F06C-6F9B-4765-A9A8-B97A4A4D5F1B}"/>
-    <hyperlink ref="A336" r:id="rId2" xr:uid="{A7D0676E-A9C0-49F9-A97A-F1E1A2A58487}"/>
-    <hyperlink ref="A335" r:id="rId3" xr:uid="{EEE6950F-3CAE-43AC-88A7-8A8ED3D8A3FB}"/>
-    <hyperlink ref="A334" r:id="rId4" xr:uid="{2F503338-110D-4200-BFDD-CA43C5BFE28C}"/>
-    <hyperlink ref="A233" r:id="rId5" xr:uid="{497AB878-023D-43CE-A035-2927AAE98B61}"/>
+    <hyperlink ref="A134" r:id="rId1" xr:uid="{3B37F06C-6F9B-4765-A9A8-B97A4A4D5F1B}"/>
+    <hyperlink ref="A301" r:id="rId2" xr:uid="{A7D0676E-A9C0-49F9-A97A-F1E1A2A58487}"/>
+    <hyperlink ref="A300" r:id="rId3" xr:uid="{EEE6950F-3CAE-43AC-88A7-8A8ED3D8A3FB}"/>
+    <hyperlink ref="A299" r:id="rId4" xr:uid="{2F503338-110D-4200-BFDD-CA43C5BFE28C}"/>
+    <hyperlink ref="A204" r:id="rId5" xr:uid="{497AB878-023D-43CE-A035-2927AAE98B61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>